<commit_message>
Add duplicate transaction check and enhance M-PESA message parsing
</commit_message>
<xml_diff>
--- a/mpesa_transactions.xlsx
+++ b/mpesa_transactions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -706,6 +706,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TI59KUQVON</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.00</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Send Money</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>FRANKLINE  ATUTI 0794492538</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5/9/25</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>8:46 PM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2505.09</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>497978.00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>TI59KUQVON Confirmed. Ksh1.00 sent to FRANKLINE  ATUTI 0794492538 on 5/9/25 at 8:46 PM. New M-PESA balance is Ksh2,505.09. Transaction cost, Ksh0.00.  Amount you can transact within the day is 497,978.00. Earn interest daily on Ziidi MMF,Dial *334#, date=1757094378914</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-09-05 20:47:47</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>